<commit_message>
changes to dup4 (add
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2940"/>
+  <dimension ref="A1:E2949"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -39016,7 +39016,7 @@
         </is>
       </c>
       <c r="E1696">
-        <v>52403</v>
+        <v>51962</v>
       </c>
     </row>
     <row r="1697">
@@ -42999,12 +42999,12 @@
       </c>
       <c r="C1880" t="inlineStr">
         <is>
-          <t>4.Ocupaci?rregular</t>
+          <t>4.Ocupación Irregularrregular</t>
         </is>
       </c>
       <c r="D1880" t="inlineStr">
         <is>
-          <t>Ocupaci?rregular</t>
+          <t>Ocupación Irregularrregular</t>
         </is>
       </c>
       <c r="E1880">
@@ -67009,6 +67009,193 @@
       </c>
       <c r="E2940">
         <v>2416</v>
+      </c>
+    </row>
+    <row r="2941">
+      <c r="A2941" t="inlineStr">
+        <is>
+          <t>cie_10</t>
+        </is>
+      </c>
+      <c r="B2941">
+        <v>1</v>
+      </c>
+      <c r="E2941">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="2942">
+      <c r="A2942" t="inlineStr">
+        <is>
+          <t>cie_10</t>
+        </is>
+      </c>
+      <c r="B2942">
+        <v>2</v>
+      </c>
+      <c r="C2942" t="inlineStr">
+        <is>
+          <t>1.Diagnosticado/a</t>
+        </is>
+      </c>
+      <c r="D2942" t="inlineStr">
+        <is>
+          <t>Diagnosticado/a</t>
+        </is>
+      </c>
+      <c r="E2942">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="2943">
+      <c r="A2943" t="inlineStr">
+        <is>
+          <t>cie_10</t>
+        </is>
+      </c>
+      <c r="B2943">
+        <v>3</v>
+      </c>
+      <c r="C2943" t="inlineStr">
+        <is>
+          <t>2.Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="D2943" t="inlineStr">
+        <is>
+          <t>Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="E2943">
+        <v>46719</v>
+      </c>
+    </row>
+    <row r="2944">
+      <c r="A2944" t="inlineStr">
+        <is>
+          <t>cie_10</t>
+        </is>
+      </c>
+      <c r="B2944">
+        <v>4</v>
+      </c>
+      <c r="C2944" t="inlineStr">
+        <is>
+          <t>3.En estudio</t>
+        </is>
+      </c>
+      <c r="D2944" t="inlineStr">
+        <is>
+          <t>En estudio</t>
+        </is>
+      </c>
+      <c r="E2944">
+        <v>20750</v>
+      </c>
+    </row>
+    <row r="2945">
+      <c r="A2945" t="inlineStr">
+        <is>
+          <t>cie_10</t>
+        </is>
+      </c>
+      <c r="B2945">
+        <v>5</v>
+      </c>
+      <c r="C2945" t="inlineStr">
+        <is>
+          <t>4.Sin información diagnóstica</t>
+        </is>
+      </c>
+      <c r="D2945" t="inlineStr">
+        <is>
+          <t>Sin información diagnóstica</t>
+        </is>
+      </c>
+      <c r="E2945">
+        <v>39930</v>
+      </c>
+    </row>
+    <row r="2946">
+      <c r="A2946" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2946">
+        <v>1</v>
+      </c>
+      <c r="E2946">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="2947">
+      <c r="A2947" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2947">
+        <v>2</v>
+      </c>
+      <c r="C2947" t="inlineStr">
+        <is>
+          <t>1.Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="D2947" t="inlineStr">
+        <is>
+          <t>Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="E2947">
+        <v>48791</v>
+      </c>
+    </row>
+    <row r="2948">
+      <c r="A2948" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2948">
+        <v>3</v>
+      </c>
+      <c r="C2948" t="inlineStr">
+        <is>
+          <t>2.En estudio</t>
+        </is>
+      </c>
+      <c r="D2948" t="inlineStr">
+        <is>
+          <t>En estudio</t>
+        </is>
+      </c>
+      <c r="E2948">
+        <v>21083</v>
+      </c>
+    </row>
+    <row r="2949">
+      <c r="A2949" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2949">
+        <v>4</v>
+      </c>
+      <c r="C2949" t="inlineStr">
+        <is>
+          <t>3.Sin información diagnóstica</t>
+        </is>
+      </c>
+      <c r="D2949" t="inlineStr">
+        <is>
+          <t>Sin información diagnóstica</t>
+        </is>
+      </c>
+      <c r="E2949">
+        <v>40529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to dup4, labels and codebook
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2949"/>
+  <dimension ref="A1:E2952"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -29054,7 +29054,7 @@
         </is>
       </c>
       <c r="E1252">
-        <v>37231</v>
+        <v>38020</v>
       </c>
     </row>
     <row r="1253">
@@ -29077,7 +29077,7 @@
         </is>
       </c>
       <c r="E1253">
-        <v>18739</v>
+        <v>17950</v>
       </c>
     </row>
     <row r="1254">
@@ -66768,7 +66768,7 @@
     <row r="2929">
       <c r="A2929" t="inlineStr">
         <is>
-          <t>obs_cambios_ninguno</t>
+          <t>abandono_temprano</t>
         </is>
       </c>
       <c r="B2929">
@@ -66781,7 +66781,7 @@
     <row r="2930">
       <c r="A2930" t="inlineStr">
         <is>
-          <t>obs_cambios_ninguno</t>
+          <t>abandono_temprano</t>
         </is>
       </c>
       <c r="B2930">
@@ -66789,22 +66789,22 @@
       </c>
       <c r="C2930" t="inlineStr">
         <is>
-          <t>1.At least 1 Change w/ the Next Entry</t>
+          <t>1.Mayor o igual a 90 días</t>
         </is>
       </c>
       <c r="D2930" t="inlineStr">
         <is>
-          <t>At least 1 Change w/ the Next Entry</t>
+          <t>Mayor o igual a 90 días</t>
         </is>
       </c>
       <c r="E2930">
-        <v>16565</v>
+        <v>83311</v>
       </c>
     </row>
     <row r="2931">
       <c r="A2931" t="inlineStr">
         <is>
-          <t>obs_cambios_ninguno</t>
+          <t>abandono_temprano</t>
         </is>
       </c>
       <c r="B2931">
@@ -66812,22 +66812,22 @@
       </c>
       <c r="C2931" t="inlineStr">
         <is>
-          <t>2.No Changes w/ the Next Entry</t>
+          <t>2.Menos de 90 días</t>
         </is>
       </c>
       <c r="D2931" t="inlineStr">
         <is>
-          <t>No Changes w/ the Next Entry</t>
+          <t>Menos de 90 días</t>
         </is>
       </c>
       <c r="E2931">
-        <v>93838</v>
+        <v>27092</v>
       </c>
     </row>
     <row r="2932">
       <c r="A2932" t="inlineStr">
         <is>
-          <t>obs_cambios_fac</t>
+          <t>obs_cambios_ninguno</t>
         </is>
       </c>
       <c r="B2932">
@@ -66840,7 +66840,7 @@
     <row r="2933">
       <c r="A2933" t="inlineStr">
         <is>
-          <t>obs_cambios_fac</t>
+          <t>obs_cambios_ninguno</t>
         </is>
       </c>
       <c r="B2933">
@@ -66848,22 +66848,22 @@
       </c>
       <c r="C2933" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.At least 1 Change w/ the Next Entry</t>
         </is>
       </c>
       <c r="D2933" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>At least 1 Change w/ the Next Entry</t>
         </is>
       </c>
       <c r="E2933">
-        <v>93838</v>
+        <v>16565</v>
       </c>
     </row>
     <row r="2934">
       <c r="A2934" t="inlineStr">
         <is>
-          <t>obs_cambios_fac</t>
+          <t>obs_cambios_ninguno</t>
         </is>
       </c>
       <c r="B2934">
@@ -66871,16 +66871,16 @@
       </c>
       <c r="C2934" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>2.No Changes w/ the Next Entry</t>
         </is>
       </c>
       <c r="D2934" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>No Changes w/ the Next Entry</t>
         </is>
       </c>
       <c r="E2934">
-        <v>5698</v>
+        <v>93838</v>
       </c>
     </row>
     <row r="2935">
@@ -66890,20 +66890,10 @@
         </is>
       </c>
       <c r="B2935">
-        <v>4</v>
-      </c>
-      <c r="C2935" t="inlineStr">
-        <is>
-          <t>3.2</t>
-        </is>
-      </c>
-      <c r="D2935" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2935">
-        <v>7801</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2936">
@@ -66913,20 +66903,20 @@
         </is>
       </c>
       <c r="B2936">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2936" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="D2936" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2936">
-        <v>2837</v>
+        <v>93838</v>
       </c>
     </row>
     <row r="2937">
@@ -66936,85 +66926,95 @@
         </is>
       </c>
       <c r="B2937">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2937" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="D2937" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2937">
-        <v>229</v>
+        <v>5698</v>
       </c>
     </row>
     <row r="2938">
       <c r="A2938" t="inlineStr">
         <is>
-          <t>centro_muj</t>
+          <t>obs_cambios_fac</t>
         </is>
       </c>
       <c r="B2938">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C2938" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="D2938" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="E2938">
-        <v>9999999</v>
+        <v>7801</v>
       </c>
     </row>
     <row r="2939">
       <c r="A2939" t="inlineStr">
         <is>
-          <t>centro_muj</t>
+          <t>obs_cambios_fac</t>
         </is>
       </c>
       <c r="B2939">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2939" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="D2939" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E2939">
-        <v>107987</v>
+        <v>2837</v>
       </c>
     </row>
     <row r="2940">
       <c r="A2940" t="inlineStr">
         <is>
-          <t>centro_muj</t>
+          <t>obs_cambios_fac</t>
         </is>
       </c>
       <c r="B2940">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2940" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="D2940" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E2940">
-        <v>2416</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2941">
       <c r="A2941" t="inlineStr">
         <is>
-          <t>cie_10</t>
+          <t>centro_muj</t>
         </is>
       </c>
       <c r="B2941">
@@ -67027,7 +67027,7 @@
     <row r="2942">
       <c r="A2942" t="inlineStr">
         <is>
-          <t>cie_10</t>
+          <t>centro_muj</t>
         </is>
       </c>
       <c r="B2942">
@@ -67035,22 +67035,22 @@
       </c>
       <c r="C2942" t="inlineStr">
         <is>
-          <t>1.Diagnosticado/a</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="D2942" t="inlineStr">
         <is>
-          <t>Diagnosticado/a</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2942">
-        <v>3004</v>
+        <v>107987</v>
       </c>
     </row>
     <row r="2943">
       <c r="A2943" t="inlineStr">
         <is>
-          <t>cie_10</t>
+          <t>centro_muj</t>
         </is>
       </c>
       <c r="B2943">
@@ -67058,16 +67058,16 @@
       </c>
       <c r="C2943" t="inlineStr">
         <is>
-          <t>2.Diagnosticado/a (1 o más)</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="D2943" t="inlineStr">
         <is>
-          <t>Diagnosticado/a (1 o más)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2943">
-        <v>46719</v>
+        <v>2416</v>
       </c>
     </row>
     <row r="2944">
@@ -67077,20 +67077,10 @@
         </is>
       </c>
       <c r="B2944">
-        <v>4</v>
-      </c>
-      <c r="C2944" t="inlineStr">
-        <is>
-          <t>3.En estudio</t>
-        </is>
-      </c>
-      <c r="D2944" t="inlineStr">
-        <is>
-          <t>En estudio</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2944">
-        <v>20750</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2945">
@@ -67100,79 +67090,89 @@
         </is>
       </c>
       <c r="B2945">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2945" t="inlineStr">
         <is>
-          <t>4.Sin información diagnóstica</t>
+          <t>1.Diagnosticado/a</t>
         </is>
       </c>
       <c r="D2945" t="inlineStr">
         <is>
-          <t>Sin información diagnóstica</t>
+          <t>Diagnosticado/a</t>
         </is>
       </c>
       <c r="E2945">
-        <v>39930</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="2946">
       <c r="A2946" t="inlineStr">
         <is>
-          <t>dsm_iv</t>
+          <t>cie_10</t>
         </is>
       </c>
       <c r="B2946">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C2946" t="inlineStr">
+        <is>
+          <t>2.Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="D2946" t="inlineStr">
+        <is>
+          <t>Diagnosticado/a (1 o más)</t>
+        </is>
       </c>
       <c r="E2946">
-        <v>9999999</v>
+        <v>46719</v>
       </c>
     </row>
     <row r="2947">
       <c r="A2947" t="inlineStr">
         <is>
-          <t>dsm_iv</t>
+          <t>cie_10</t>
         </is>
       </c>
       <c r="B2947">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2947" t="inlineStr">
         <is>
-          <t>1.Diagnosticado/a (1 o más)</t>
+          <t>3.En estudio</t>
         </is>
       </c>
       <c r="D2947" t="inlineStr">
         <is>
-          <t>Diagnosticado/a (1 o más)</t>
+          <t>En estudio</t>
         </is>
       </c>
       <c r="E2947">
-        <v>48791</v>
+        <v>20750</v>
       </c>
     </row>
     <row r="2948">
       <c r="A2948" t="inlineStr">
         <is>
-          <t>dsm_iv</t>
+          <t>cie_10</t>
         </is>
       </c>
       <c r="B2948">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2948" t="inlineStr">
         <is>
-          <t>2.En estudio</t>
+          <t>4.Sin información diagnóstica</t>
         </is>
       </c>
       <c r="D2948" t="inlineStr">
         <is>
-          <t>En estudio</t>
+          <t>Sin información diagnóstica</t>
         </is>
       </c>
       <c r="E2948">
-        <v>21083</v>
+        <v>39930</v>
       </c>
     </row>
     <row r="2949">
@@ -67182,19 +67182,78 @@
         </is>
       </c>
       <c r="B2949">
+        <v>1</v>
+      </c>
+      <c r="E2949">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="2950">
+      <c r="A2950" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2950">
+        <v>2</v>
+      </c>
+      <c r="C2950" t="inlineStr">
+        <is>
+          <t>1.Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="D2950" t="inlineStr">
+        <is>
+          <t>Diagnosticado/a (1 o más)</t>
+        </is>
+      </c>
+      <c r="E2950">
+        <v>48791</v>
+      </c>
+    </row>
+    <row r="2951">
+      <c r="A2951" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2951">
+        <v>3</v>
+      </c>
+      <c r="C2951" t="inlineStr">
+        <is>
+          <t>2.En estudio</t>
+        </is>
+      </c>
+      <c r="D2951" t="inlineStr">
+        <is>
+          <t>En estudio</t>
+        </is>
+      </c>
+      <c r="E2951">
+        <v>21083</v>
+      </c>
+    </row>
+    <row r="2952">
+      <c r="A2952" t="inlineStr">
+        <is>
+          <t>dsm_iv</t>
+        </is>
+      </c>
+      <c r="B2952">
         <v>4</v>
       </c>
-      <c r="C2949" t="inlineStr">
+      <c r="C2952" t="inlineStr">
         <is>
           <t>3.Sin información diagnóstica</t>
         </is>
       </c>
-      <c r="D2949" t="inlineStr">
+      <c r="D2952" t="inlineStr">
         <is>
           <t>Sin información diagnóstica</t>
         </is>
       </c>
-      <c r="E2949">
+      <c r="E2952">
         <v>40529</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to descriptives & codebook, in wide information (days in treatment, diff between days and mean values), changes to via_adm_sus_prin, cat_ocupacional and status_ocupacional, and some requirements of joel, creating sept 2020 db. This db has an arrangement from hash_key and fech_ing, from the latest to the earliest treatment for each user. git push
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -41619,7 +41619,7 @@
         </is>
       </c>
       <c r="E1817">
-        <v>39711</v>
+        <v>39188</v>
       </c>
     </row>
     <row r="1818">
@@ -41642,7 +41642,7 @@
         </is>
       </c>
       <c r="E1818">
-        <v>50638</v>
+        <v>51348</v>
       </c>
     </row>
     <row r="1819">
@@ -41665,7 +41665,7 @@
         </is>
       </c>
       <c r="E1819">
-        <v>19406</v>
+        <v>19219</v>
       </c>
     </row>
     <row r="1820">

</xml_diff>

<commit_message>
changes to Descriptives (sus_ini_mvv), added Matching Process, changed codebook
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -67173,7 +67173,7 @@
         </is>
       </c>
       <c r="E2955">
-        <v>61441</v>
+        <v>59319</v>
       </c>
     </row>
     <row r="2956">
@@ -67196,7 +67196,7 @@
         </is>
       </c>
       <c r="E2956">
-        <v>3966</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="2957">
@@ -67219,7 +67219,7 @@
         </is>
       </c>
       <c r="E2957">
-        <v>29843</v>
+        <v>31074</v>
       </c>
     </row>
     <row r="2958">
@@ -67242,7 +67242,7 @@
         </is>
       </c>
       <c r="E2958">
-        <v>2789</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="2959">
@@ -67265,7 +67265,7 @@
         </is>
       </c>
       <c r="E2959">
-        <v>5084</v>
+        <v>5834</v>
       </c>
     </row>
     <row r="2960">

</xml_diff>

<commit_message>
changes into occupational condition, solution of duplicated cumulative difference wide 1:10 in the last one, and part of the matching process
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3020"/>
+  <dimension ref="A1:E3034"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -68471,6 +68471,308 @@
         <v>27868</v>
       </c>
     </row>
+    <row r="3021">
+      <c r="A3021" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3021">
+        <v>1</v>
+      </c>
+      <c r="E3021">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="3022">
+      <c r="A3022" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3022">
+        <v>2</v>
+      </c>
+      <c r="C3022" t="inlineStr">
+        <is>
+          <t>1.Employed</t>
+        </is>
+      </c>
+      <c r="D3022" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+      <c r="E3022">
+        <v>50394</v>
+      </c>
+    </row>
+    <row r="3023">
+      <c r="A3023" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3023">
+        <v>3</v>
+      </c>
+      <c r="C3023" t="inlineStr">
+        <is>
+          <t>2.Inactive</t>
+        </is>
+      </c>
+      <c r="D3023" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+      <c r="E3023">
+        <v>11485</v>
+      </c>
+    </row>
+    <row r="3024">
+      <c r="A3024" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3024">
+        <v>4</v>
+      </c>
+      <c r="C3024" t="inlineStr">
+        <is>
+          <t>3.Looking for a job for the first time</t>
+        </is>
+      </c>
+      <c r="D3024" t="inlineStr">
+        <is>
+          <t>Looking for a job for the first time</t>
+        </is>
+      </c>
+      <c r="E3024">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3025">
+      <c r="A3025" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3025">
+        <v>5</v>
+      </c>
+      <c r="C3025" t="inlineStr">
+        <is>
+          <t>4.No activity</t>
+        </is>
+      </c>
+      <c r="D3025" t="inlineStr">
+        <is>
+          <t>No activity</t>
+        </is>
+      </c>
+      <c r="E3025">
+        <v>6811</v>
+      </c>
+    </row>
+    <row r="3026">
+      <c r="A3026" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3026">
+        <v>6</v>
+      </c>
+      <c r="C3026" t="inlineStr">
+        <is>
+          <t>5.Not seeking for work</t>
+        </is>
+      </c>
+      <c r="D3026" t="inlineStr">
+        <is>
+          <t>Not seeking for work</t>
+        </is>
+      </c>
+      <c r="E3026">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="3027">
+      <c r="A3027" t="inlineStr">
+        <is>
+          <t>condicion_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3027">
+        <v>7</v>
+      </c>
+      <c r="C3027" t="inlineStr">
+        <is>
+          <t>6.Unemployed</t>
+        </is>
+      </c>
+      <c r="D3027" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
+      </c>
+      <c r="E3027">
+        <v>39676</v>
+      </c>
+    </row>
+    <row r="3028">
+      <c r="A3028" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3028">
+        <v>1</v>
+      </c>
+      <c r="E3028">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="3029">
+      <c r="A3029" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3029">
+        <v>2</v>
+      </c>
+      <c r="C3029" t="inlineStr">
+        <is>
+          <t>1.Employer</t>
+        </is>
+      </c>
+      <c r="D3029" t="inlineStr">
+        <is>
+          <t>Employer</t>
+        </is>
+      </c>
+      <c r="E3029">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="3030">
+      <c r="A3030" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3030">
+        <v>3</v>
+      </c>
+      <c r="C3030" t="inlineStr">
+        <is>
+          <t>2.Other</t>
+        </is>
+      </c>
+      <c r="D3030" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="E3030">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="3031">
+      <c r="A3031" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3031">
+        <v>4</v>
+      </c>
+      <c r="C3031" t="inlineStr">
+        <is>
+          <t>3.Salaried</t>
+        </is>
+      </c>
+      <c r="D3031" t="inlineStr">
+        <is>
+          <t>Salaried</t>
+        </is>
+      </c>
+      <c r="E3031">
+        <v>30140</v>
+      </c>
+    </row>
+    <row r="3032">
+      <c r="A3032" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3032">
+        <v>5</v>
+      </c>
+      <c r="C3032" t="inlineStr">
+        <is>
+          <t>4.Self-employed</t>
+        </is>
+      </c>
+      <c r="D3032" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+      <c r="E3032">
+        <v>13466</v>
+      </c>
+    </row>
+    <row r="3033">
+      <c r="A3033" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3033">
+        <v>6</v>
+      </c>
+      <c r="C3033" t="inlineStr">
+        <is>
+          <t>5.Unpaid family labour</t>
+        </is>
+      </c>
+      <c r="D3033" t="inlineStr">
+        <is>
+          <t>Unpaid family labour</t>
+        </is>
+      </c>
+      <c r="E3033">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3034">
+      <c r="A3034" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3034">
+        <v>7</v>
+      </c>
+      <c r="C3034" t="inlineStr">
+        <is>
+          <t>6.Volunteer worker</t>
+        </is>
+      </c>
+      <c r="D3034" t="inlineStr">
+        <is>
+          <t>Volunteer worker</t>
+        </is>
+      </c>
+      <c r="E3034">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in codebook, solution of inconsistencies between age of onset of drug use and age of onset of drug use in the primary substance and the age of admission (since Duplicates4), modification of Matching process to include Survival setting, and creation of another rmd
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -55767,7 +55767,7 @@
         </is>
       </c>
       <c r="E2443">
-        <v>30327</v>
+        <v>27184</v>
       </c>
     </row>
     <row r="2444">
@@ -55790,7 +55790,7 @@
         </is>
       </c>
       <c r="E2444">
-        <v>24589</v>
+        <v>22279</v>
       </c>
     </row>
     <row r="2445">
@@ -55813,7 +55813,7 @@
         </is>
       </c>
       <c r="E2445">
-        <v>28698</v>
+        <v>26399</v>
       </c>
     </row>
     <row r="2446">
@@ -55836,7 +55836,7 @@
         </is>
       </c>
       <c r="E2446">
-        <v>25190</v>
+        <v>23218</v>
       </c>
     </row>
     <row r="2447">
@@ -67091,7 +67091,7 @@
         </is>
       </c>
       <c r="E2951">
-        <v>35335</v>
+        <v>59545</v>
       </c>
     </row>
     <row r="2952">
@@ -67114,7 +67114,7 @@
         </is>
       </c>
       <c r="E2952">
-        <v>48914</v>
+        <v>11834</v>
       </c>
     </row>
     <row r="2953">
@@ -67137,7 +67137,7 @@
         </is>
       </c>
       <c r="E2953">
-        <v>25507</v>
+        <v>38377</v>
       </c>
     </row>
     <row r="2954">

</xml_diff>

<commit_message>
changes to dates of discharge that exceeded 2019-11-13, correction of codebooks and Desc. Additionally, Matching Process is in completition state.
</commit_message>
<xml_diff>
--- a/labels_codebook.xlsx
+++ b/labels_codebook.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3034"/>
+  <dimension ref="A1:E3037"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -66979,7 +66979,7 @@
     <row r="2946">
       <c r="A2946" t="inlineStr">
         <is>
-          <t>dg_cie_10_rec</t>
+          <t>dias_trat_alta_temprana</t>
         </is>
       </c>
       <c r="B2946">
@@ -66992,7 +66992,7 @@
     <row r="2947">
       <c r="A2947" t="inlineStr">
         <is>
-          <t>dg_cie_10_rec</t>
+          <t>dias_trat_alta_temprana</t>
         </is>
       </c>
       <c r="B2947">
@@ -67000,22 +67000,22 @@
       </c>
       <c r="C2947" t="inlineStr">
         <is>
-          <t>1.Without psychiatric comorbidity</t>
+          <t>1.Mayor o igual a 90 días</t>
         </is>
       </c>
       <c r="D2947" t="inlineStr">
         <is>
-          <t>Without psychiatric comorbidity</t>
+          <t>Mayor o igual a 90 días</t>
         </is>
       </c>
       <c r="E2947">
-        <v>39695</v>
+        <v>82664</v>
       </c>
     </row>
     <row r="2948">
       <c r="A2948" t="inlineStr">
         <is>
-          <t>dg_cie_10_rec</t>
+          <t>dias_trat_alta_temprana</t>
         </is>
       </c>
       <c r="B2948">
@@ -67023,16 +67023,16 @@
       </c>
       <c r="C2948" t="inlineStr">
         <is>
-          <t>2.Diagnosis unknown (under study)</t>
+          <t>2.Menos de 90 días</t>
         </is>
       </c>
       <c r="D2948" t="inlineStr">
         <is>
-          <t>Diagnosis unknown (under study)</t>
+          <t>Menos de 90 días</t>
         </is>
       </c>
       <c r="E2948">
-        <v>20723</v>
+        <v>27092</v>
       </c>
     </row>
     <row r="2949">
@@ -67042,47 +67042,47 @@
         </is>
       </c>
       <c r="B2949">
-        <v>4</v>
-      </c>
-      <c r="C2949" t="inlineStr">
-        <is>
-          <t>3.With psychiatric comorbidity</t>
-        </is>
-      </c>
-      <c r="D2949" t="inlineStr">
-        <is>
-          <t>With psychiatric comorbidity</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2949">
-        <v>49338</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2950">
       <c r="A2950" t="inlineStr">
         <is>
-          <t>dg_dsm_iv_rec</t>
+          <t>dg_cie_10_rec</t>
         </is>
       </c>
       <c r="B2950">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2950" t="inlineStr">
+        <is>
+          <t>1.Without psychiatric comorbidity</t>
+        </is>
+      </c>
+      <c r="D2950" t="inlineStr">
+        <is>
+          <t>Without psychiatric comorbidity</t>
+        </is>
       </c>
       <c r="E2950">
-        <v>9999999</v>
+        <v>39695</v>
       </c>
     </row>
     <row r="2951">
       <c r="A2951" t="inlineStr">
         <is>
-          <t>dg_dsm_iv_rec</t>
+          <t>dg_cie_10_rec</t>
         </is>
       </c>
       <c r="B2951">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2951" t="inlineStr">
         <is>
-          <t>1.Diagnosis unknown (under study)</t>
+          <t>2.Diagnosis unknown (under study)</t>
         </is>
       </c>
       <c r="D2951" t="inlineStr">
@@ -67091,21 +67091,21 @@
         </is>
       </c>
       <c r="E2951">
-        <v>59545</v>
+        <v>20723</v>
       </c>
     </row>
     <row r="2952">
       <c r="A2952" t="inlineStr">
         <is>
-          <t>dg_dsm_iv_rec</t>
+          <t>dg_cie_10_rec</t>
         </is>
       </c>
       <c r="B2952">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2952" t="inlineStr">
         <is>
-          <t>2.With psychiatric comorbidity</t>
+          <t>3.With psychiatric comorbidity</t>
         </is>
       </c>
       <c r="D2952" t="inlineStr">
@@ -67114,7 +67114,7 @@
         </is>
       </c>
       <c r="E2952">
-        <v>11834</v>
+        <v>49338</v>
       </c>
     </row>
     <row r="2953">
@@ -67124,79 +67124,79 @@
         </is>
       </c>
       <c r="B2953">
-        <v>4</v>
-      </c>
-      <c r="C2953" t="inlineStr">
-        <is>
-          <t>3.Without psychiatric comorbidity</t>
-        </is>
-      </c>
-      <c r="D2953" t="inlineStr">
-        <is>
-          <t>Without psychiatric comorbidity</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2953">
-        <v>38377</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2954">
       <c r="A2954" t="inlineStr">
         <is>
-          <t>sus_ini_mod_mvv</t>
+          <t>dg_dsm_iv_rec</t>
         </is>
       </c>
       <c r="B2954">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2954" t="inlineStr">
+        <is>
+          <t>1.Diagnosis unknown (under study)</t>
+        </is>
+      </c>
+      <c r="D2954" t="inlineStr">
+        <is>
+          <t>Diagnosis unknown (under study)</t>
+        </is>
       </c>
       <c r="E2954">
-        <v>9999999</v>
+        <v>59545</v>
       </c>
     </row>
     <row r="2955">
       <c r="A2955" t="inlineStr">
         <is>
-          <t>sus_ini_mod_mvv</t>
+          <t>dg_dsm_iv_rec</t>
         </is>
       </c>
       <c r="B2955">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2955" t="inlineStr">
         <is>
-          <t>1.Alcohol</t>
+          <t>2.With psychiatric comorbidity</t>
         </is>
       </c>
       <c r="D2955" t="inlineStr">
         <is>
-          <t>Alcohol</t>
+          <t>With psychiatric comorbidity</t>
         </is>
       </c>
       <c r="E2955">
-        <v>59319</v>
+        <v>11834</v>
       </c>
     </row>
     <row r="2956">
       <c r="A2956" t="inlineStr">
         <is>
-          <t>sus_ini_mod_mvv</t>
+          <t>dg_dsm_iv_rec</t>
         </is>
       </c>
       <c r="B2956">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2956" t="inlineStr">
         <is>
-          <t>2.Cocaine hydrochloride</t>
+          <t>3.Without psychiatric comorbidity</t>
         </is>
       </c>
       <c r="D2956" t="inlineStr">
         <is>
-          <t>Cocaine hydrochloride</t>
+          <t>Without psychiatric comorbidity</t>
         </is>
       </c>
       <c r="E2956">
-        <v>4350</v>
+        <v>38377</v>
       </c>
     </row>
     <row r="2957">
@@ -67206,20 +67206,10 @@
         </is>
       </c>
       <c r="B2957">
-        <v>4</v>
-      </c>
-      <c r="C2957" t="inlineStr">
-        <is>
-          <t>3.Marijuana</t>
-        </is>
-      </c>
-      <c r="D2957" t="inlineStr">
-        <is>
-          <t>Marijuana</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2957">
-        <v>31074</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2958">
@@ -67229,20 +67219,20 @@
         </is>
       </c>
       <c r="B2958">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2958" t="inlineStr">
         <is>
-          <t>4.Other</t>
+          <t>1.Alcohol</t>
         </is>
       </c>
       <c r="D2958" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Alcohol</t>
         </is>
       </c>
       <c r="E2958">
-        <v>2546</v>
+        <v>59319</v>
       </c>
     </row>
     <row r="2959">
@@ -67252,79 +67242,89 @@
         </is>
       </c>
       <c r="B2959">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2959" t="inlineStr">
         <is>
-          <t>5.Cocaine paste</t>
+          <t>2.Cocaine hydrochloride</t>
         </is>
       </c>
       <c r="D2959" t="inlineStr">
         <is>
-          <t>Cocaine paste</t>
+          <t>Cocaine hydrochloride</t>
         </is>
       </c>
       <c r="E2959">
-        <v>5834</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="2960">
       <c r="A2960" t="inlineStr">
         <is>
-          <t>estatus_ocupacional_rec</t>
+          <t>sus_ini_mod_mvv</t>
         </is>
       </c>
       <c r="B2960">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C2960" t="inlineStr">
+        <is>
+          <t>3.Marijuana</t>
+        </is>
+      </c>
+      <c r="D2960" t="inlineStr">
+        <is>
+          <t>Marijuana</t>
+        </is>
       </c>
       <c r="E2960">
-        <v>9999999</v>
+        <v>31074</v>
       </c>
     </row>
     <row r="2961">
       <c r="A2961" t="inlineStr">
         <is>
-          <t>estatus_ocupacional_rec</t>
+          <t>sus_ini_mod_mvv</t>
         </is>
       </c>
       <c r="B2961">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2961" t="inlineStr">
         <is>
-          <t>1.Unemployed</t>
+          <t>4.Other</t>
         </is>
       </c>
       <c r="D2961" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E2961">
-        <v>39188</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="2962">
       <c r="A2962" t="inlineStr">
         <is>
-          <t>estatus_ocupacional_rec</t>
+          <t>sus_ini_mod_mvv</t>
         </is>
       </c>
       <c r="B2962">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2962" t="inlineStr">
         <is>
-          <t>2.Employed</t>
+          <t>5.Cocaine paste</t>
         </is>
       </c>
       <c r="D2962" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Cocaine paste</t>
         </is>
       </c>
       <c r="E2962">
-        <v>51348</v>
+        <v>5834</v>
       </c>
     </row>
     <row r="2963">
@@ -67334,85 +67334,85 @@
         </is>
       </c>
       <c r="B2963">
-        <v>4</v>
-      </c>
-      <c r="C2963" t="inlineStr">
-        <is>
-          <t>3.Inactive</t>
-        </is>
-      </c>
-      <c r="D2963" t="inlineStr">
-        <is>
-          <t>Inactive</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E2963">
-        <v>19219</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="2964">
       <c r="A2964" t="inlineStr">
         <is>
-          <t>hijos_trat_res</t>
+          <t>estatus_ocupacional_rec</t>
         </is>
       </c>
       <c r="B2964">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2964" t="inlineStr">
+        <is>
+          <t>1.Unemployed</t>
+        </is>
+      </c>
+      <c r="D2964" t="inlineStr">
+        <is>
+          <t>Unemployed</t>
+        </is>
       </c>
       <c r="E2964">
-        <v>9999999</v>
+        <v>39188</v>
       </c>
     </row>
     <row r="2965">
       <c r="A2965" t="inlineStr">
         <is>
-          <t>hijos_trat_res</t>
+          <t>estatus_ocupacional_rec</t>
         </is>
       </c>
       <c r="B2965">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2965" t="inlineStr">
         <is>
-          <t>1.Did not had children in treatment</t>
+          <t>2.Employed</t>
         </is>
       </c>
       <c r="D2965" t="inlineStr">
         <is>
-          <t>Did not had children in treatment</t>
+          <t>Employed</t>
         </is>
       </c>
       <c r="E2965">
-        <v>95656</v>
+        <v>51348</v>
       </c>
     </row>
     <row r="2966">
       <c r="A2966" t="inlineStr">
         <is>
-          <t>hijos_trat_res</t>
+          <t>estatus_ocupacional_rec</t>
         </is>
       </c>
       <c r="B2966">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2966" t="inlineStr">
         <is>
-          <t>2.Had children in treatments</t>
+          <t>3.Inactive</t>
         </is>
       </c>
       <c r="D2966" t="inlineStr">
         <is>
-          <t>Had children in treatments</t>
+          <t>Inactive</t>
         </is>
       </c>
       <c r="E2966">
-        <v>1653</v>
+        <v>19219</v>
       </c>
     </row>
     <row r="2967">
       <c r="A2967" t="inlineStr">
         <is>
-          <t>dg_fis_anemia</t>
+          <t>hijos_trat_res</t>
         </is>
       </c>
       <c r="B2967">
@@ -67425,7 +67425,7 @@
     <row r="2968">
       <c r="A2968" t="inlineStr">
         <is>
-          <t>dg_fis_anemia</t>
+          <t>hijos_trat_res</t>
         </is>
       </c>
       <c r="B2968">
@@ -67433,22 +67433,22 @@
       </c>
       <c r="C2968" t="inlineStr">
         <is>
-          <t>1.Absence</t>
+          <t>1.Did not had children in treatment</t>
         </is>
       </c>
       <c r="D2968" t="inlineStr">
         <is>
-          <t>Absence</t>
+          <t>Did not had children in treatment</t>
         </is>
       </c>
       <c r="E2968">
-        <v>109650</v>
+        <v>95656</v>
       </c>
     </row>
     <row r="2969">
       <c r="A2969" t="inlineStr">
         <is>
-          <t>dg_fis_anemia</t>
+          <t>hijos_trat_res</t>
         </is>
       </c>
       <c r="B2969">
@@ -67456,22 +67456,22 @@
       </c>
       <c r="C2969" t="inlineStr">
         <is>
-          <t>2.Presence</t>
+          <t>2.Had children in treatments</t>
         </is>
       </c>
       <c r="D2969" t="inlineStr">
         <is>
-          <t>Presence</t>
+          <t>Had children in treatments</t>
         </is>
       </c>
       <c r="E2969">
-        <v>106</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="2970">
       <c r="A2970" t="inlineStr">
         <is>
-          <t>dg_fis_card</t>
+          <t>dg_fis_anemia</t>
         </is>
       </c>
       <c r="B2970">
@@ -67484,7 +67484,7 @@
     <row r="2971">
       <c r="A2971" t="inlineStr">
         <is>
-          <t>dg_fis_card</t>
+          <t>dg_fis_anemia</t>
         </is>
       </c>
       <c r="B2971">
@@ -67501,13 +67501,13 @@
         </is>
       </c>
       <c r="E2971">
-        <v>108644</v>
+        <v>109650</v>
       </c>
     </row>
     <row r="2972">
       <c r="A2972" t="inlineStr">
         <is>
-          <t>dg_fis_card</t>
+          <t>dg_fis_anemia</t>
         </is>
       </c>
       <c r="B2972">
@@ -67524,13 +67524,13 @@
         </is>
       </c>
       <c r="E2972">
-        <v>1112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2973">
       <c r="A2973" t="inlineStr">
         <is>
-          <t>dg_fis_in_study</t>
+          <t>dg_fis_card</t>
         </is>
       </c>
       <c r="B2973">
@@ -67543,7 +67543,7 @@
     <row r="2974">
       <c r="A2974" t="inlineStr">
         <is>
-          <t>dg_fis_in_study</t>
+          <t>dg_fis_card</t>
         </is>
       </c>
       <c r="B2974">
@@ -67560,13 +67560,13 @@
         </is>
       </c>
       <c r="E2974">
-        <v>50839</v>
+        <v>108644</v>
       </c>
     </row>
     <row r="2975">
       <c r="A2975" t="inlineStr">
         <is>
-          <t>dg_fis_in_study</t>
+          <t>dg_fis_card</t>
         </is>
       </c>
       <c r="B2975">
@@ -67583,13 +67583,13 @@
         </is>
       </c>
       <c r="E2975">
-        <v>58917</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="2976">
       <c r="A2976" t="inlineStr">
         <is>
-          <t>dg_fis_enf_som</t>
+          <t>dg_fis_in_study</t>
         </is>
       </c>
       <c r="B2976">
@@ -67602,7 +67602,7 @@
     <row r="2977">
       <c r="A2977" t="inlineStr">
         <is>
-          <t>dg_fis_enf_som</t>
+          <t>dg_fis_in_study</t>
         </is>
       </c>
       <c r="B2977">
@@ -67619,13 +67619,13 @@
         </is>
       </c>
       <c r="E2977">
-        <v>108970</v>
+        <v>50839</v>
       </c>
     </row>
     <row r="2978">
       <c r="A2978" t="inlineStr">
         <is>
-          <t>dg_fis_enf_som</t>
+          <t>dg_fis_in_study</t>
         </is>
       </c>
       <c r="B2978">
@@ -67642,13 +67642,13 @@
         </is>
       </c>
       <c r="E2978">
-        <v>786</v>
+        <v>58917</v>
       </c>
     </row>
     <row r="2979">
       <c r="A2979" t="inlineStr">
         <is>
-          <t>dg_fis_ets</t>
+          <t>dg_fis_enf_som</t>
         </is>
       </c>
       <c r="B2979">
@@ -67661,7 +67661,7 @@
     <row r="2980">
       <c r="A2980" t="inlineStr">
         <is>
-          <t>dg_fis_ets</t>
+          <t>dg_fis_enf_som</t>
         </is>
       </c>
       <c r="B2980">
@@ -67678,13 +67678,13 @@
         </is>
       </c>
       <c r="E2980">
-        <v>109045</v>
+        <v>108970</v>
       </c>
     </row>
     <row r="2981">
       <c r="A2981" t="inlineStr">
         <is>
-          <t>dg_fis_ets</t>
+          <t>dg_fis_enf_som</t>
         </is>
       </c>
       <c r="B2981">
@@ -67701,13 +67701,13 @@
         </is>
       </c>
       <c r="E2981">
-        <v>711</v>
+        <v>786</v>
       </c>
     </row>
     <row r="2982">
       <c r="A2982" t="inlineStr">
         <is>
-          <t>dg_fis_hep_alc</t>
+          <t>dg_fis_ets</t>
         </is>
       </c>
       <c r="B2982">
@@ -67720,7 +67720,7 @@
     <row r="2983">
       <c r="A2983" t="inlineStr">
         <is>
-          <t>dg_fis_hep_alc</t>
+          <t>dg_fis_ets</t>
         </is>
       </c>
       <c r="B2983">
@@ -67737,13 +67737,13 @@
         </is>
       </c>
       <c r="E2983">
-        <v>109428</v>
+        <v>109045</v>
       </c>
     </row>
     <row r="2984">
       <c r="A2984" t="inlineStr">
         <is>
-          <t>dg_fis_hep_alc</t>
+          <t>dg_fis_ets</t>
         </is>
       </c>
       <c r="B2984">
@@ -67760,13 +67760,13 @@
         </is>
       </c>
       <c r="E2984">
-        <v>328</v>
+        <v>711</v>
       </c>
     </row>
     <row r="2985">
       <c r="A2985" t="inlineStr">
         <is>
-          <t>dg_fis_hep_b</t>
+          <t>dg_fis_hep_alc</t>
         </is>
       </c>
       <c r="B2985">
@@ -67779,7 +67779,7 @@
     <row r="2986">
       <c r="A2986" t="inlineStr">
         <is>
-          <t>dg_fis_hep_b</t>
+          <t>dg_fis_hep_alc</t>
         </is>
       </c>
       <c r="B2986">
@@ -67796,13 +67796,13 @@
         </is>
       </c>
       <c r="E2986">
-        <v>109638</v>
+        <v>109428</v>
       </c>
     </row>
     <row r="2987">
       <c r="A2987" t="inlineStr">
         <is>
-          <t>dg_fis_hep_b</t>
+          <t>dg_fis_hep_alc</t>
         </is>
       </c>
       <c r="B2987">
@@ -67819,13 +67819,13 @@
         </is>
       </c>
       <c r="E2987">
-        <v>118</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2988">
       <c r="A2988" t="inlineStr">
         <is>
-          <t>dg_fis_hep_cro</t>
+          <t>dg_fis_hep_b</t>
         </is>
       </c>
       <c r="B2988">
@@ -67838,7 +67838,7 @@
     <row r="2989">
       <c r="A2989" t="inlineStr">
         <is>
-          <t>dg_fis_hep_cro</t>
+          <t>dg_fis_hep_b</t>
         </is>
       </c>
       <c r="B2989">
@@ -67855,13 +67855,13 @@
         </is>
       </c>
       <c r="E2989">
-        <v>109629</v>
+        <v>109638</v>
       </c>
     </row>
     <row r="2990">
       <c r="A2990" t="inlineStr">
         <is>
-          <t>dg_fis_hep_cro</t>
+          <t>dg_fis_hep_b</t>
         </is>
       </c>
       <c r="B2990">
@@ -67878,13 +67878,13 @@
         </is>
       </c>
       <c r="E2990">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2991">
       <c r="A2991" t="inlineStr">
         <is>
-          <t>dg_fis_inf</t>
+          <t>dg_fis_hep_cro</t>
         </is>
       </c>
       <c r="B2991">
@@ -67897,7 +67897,7 @@
     <row r="2992">
       <c r="A2992" t="inlineStr">
         <is>
-          <t>dg_fis_inf</t>
+          <t>dg_fis_hep_cro</t>
         </is>
       </c>
       <c r="B2992">
@@ -67914,13 +67914,13 @@
         </is>
       </c>
       <c r="E2992">
-        <v>109598</v>
+        <v>109629</v>
       </c>
     </row>
     <row r="2993">
       <c r="A2993" t="inlineStr">
         <is>
-          <t>dg_fis_inf</t>
+          <t>dg_fis_hep_cro</t>
         </is>
       </c>
       <c r="B2993">
@@ -67937,13 +67937,13 @@
         </is>
       </c>
       <c r="E2993">
-        <v>158</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2994">
       <c r="A2994" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis_ries_vit</t>
+          <t>dg_fis_inf</t>
         </is>
       </c>
       <c r="B2994">
@@ -67956,7 +67956,7 @@
     <row r="2995">
       <c r="A2995" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis_ries_vit</t>
+          <t>dg_fis_inf</t>
         </is>
       </c>
       <c r="B2995">
@@ -67973,13 +67973,13 @@
         </is>
       </c>
       <c r="E2995">
-        <v>108371</v>
+        <v>109598</v>
       </c>
     </row>
     <row r="2996">
       <c r="A2996" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis_ries_vit</t>
+          <t>dg_fis_inf</t>
         </is>
       </c>
       <c r="B2996">
@@ -67996,13 +67996,13 @@
         </is>
       </c>
       <c r="E2996">
-        <v>1385</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2997">
       <c r="A2997" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis</t>
+          <t>dg_fis_otr_cond_fis_ries_vit</t>
         </is>
       </c>
       <c r="B2997">
@@ -68015,7 +68015,7 @@
     <row r="2998">
       <c r="A2998" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis</t>
+          <t>dg_fis_otr_cond_fis_ries_vit</t>
         </is>
       </c>
       <c r="B2998">
@@ -68032,13 +68032,13 @@
         </is>
       </c>
       <c r="E2998">
-        <v>106800</v>
+        <v>108371</v>
       </c>
     </row>
     <row r="2999">
       <c r="A2999" t="inlineStr">
         <is>
-          <t>dg_fis_otr_cond_fis</t>
+          <t>dg_fis_otr_cond_fis_ries_vit</t>
         </is>
       </c>
       <c r="B2999">
@@ -68055,13 +68055,13 @@
         </is>
       </c>
       <c r="E2999">
-        <v>2956</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="3000">
       <c r="A3000" t="inlineStr">
         <is>
-          <t>dg_fis_pat_buc</t>
+          <t>dg_fis_otr_cond_fis</t>
         </is>
       </c>
       <c r="B3000">
@@ -68074,7 +68074,7 @@
     <row r="3001">
       <c r="A3001" t="inlineStr">
         <is>
-          <t>dg_fis_pat_buc</t>
+          <t>dg_fis_otr_cond_fis</t>
         </is>
       </c>
       <c r="B3001">
@@ -68091,13 +68091,13 @@
         </is>
       </c>
       <c r="E3001">
-        <v>108205</v>
+        <v>106800</v>
       </c>
     </row>
     <row r="3002">
       <c r="A3002" t="inlineStr">
         <is>
-          <t>dg_fis_pat_buc</t>
+          <t>dg_fis_otr_cond_fis</t>
         </is>
       </c>
       <c r="B3002">
@@ -68114,13 +68114,13 @@
         </is>
       </c>
       <c r="E3002">
-        <v>1551</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="3003">
       <c r="A3003" t="inlineStr">
         <is>
-          <t>dg_fis_pat_ges_intrau</t>
+          <t>dg_fis_pat_buc</t>
         </is>
       </c>
       <c r="B3003">
@@ -68133,7 +68133,7 @@
     <row r="3004">
       <c r="A3004" t="inlineStr">
         <is>
-          <t>dg_fis_pat_ges_intrau</t>
+          <t>dg_fis_pat_buc</t>
         </is>
       </c>
       <c r="B3004">
@@ -68150,13 +68150,13 @@
         </is>
       </c>
       <c r="E3004">
-        <v>109672</v>
+        <v>108205</v>
       </c>
     </row>
     <row r="3005">
       <c r="A3005" t="inlineStr">
         <is>
-          <t>dg_fis_pat_ges_intrau</t>
+          <t>dg_fis_pat_buc</t>
         </is>
       </c>
       <c r="B3005">
@@ -68173,13 +68173,13 @@
         </is>
       </c>
       <c r="E3005">
-        <v>84</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="3006">
       <c r="A3006" t="inlineStr">
         <is>
-          <t>dg_fis_trau_sec</t>
+          <t>dg_fis_pat_ges_intrau</t>
         </is>
       </c>
       <c r="B3006">
@@ -68192,7 +68192,7 @@
     <row r="3007">
       <c r="A3007" t="inlineStr">
         <is>
-          <t>dg_fis_trau_sec</t>
+          <t>dg_fis_pat_ges_intrau</t>
         </is>
       </c>
       <c r="B3007">
@@ -68209,13 +68209,13 @@
         </is>
       </c>
       <c r="E3007">
-        <v>107938</v>
+        <v>109672</v>
       </c>
     </row>
     <row r="3008">
       <c r="A3008" t="inlineStr">
         <is>
-          <t>dg_fis_trau_sec</t>
+          <t>dg_fis_pat_ges_intrau</t>
         </is>
       </c>
       <c r="B3008">
@@ -68232,13 +68232,13 @@
         </is>
       </c>
       <c r="E3008">
-        <v>1818</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3009">
       <c r="A3009" t="inlineStr">
         <is>
-          <t>otros_pr_sm_abu_sex</t>
+          <t>dg_fis_trau_sec</t>
         </is>
       </c>
       <c r="B3009">
@@ -68251,7 +68251,7 @@
     <row r="3010">
       <c r="A3010" t="inlineStr">
         <is>
-          <t>otros_pr_sm_abu_sex</t>
+          <t>dg_fis_trau_sec</t>
         </is>
       </c>
       <c r="B3010">
@@ -68268,13 +68268,13 @@
         </is>
       </c>
       <c r="E3010">
-        <v>107666</v>
+        <v>107938</v>
       </c>
     </row>
     <row r="3011">
       <c r="A3011" t="inlineStr">
         <is>
-          <t>otros_pr_sm_abu_sex</t>
+          <t>dg_fis_trau_sec</t>
         </is>
       </c>
       <c r="B3011">
@@ -68291,13 +68291,13 @@
         </is>
       </c>
       <c r="E3011">
-        <v>2090</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="3012">
       <c r="A3012" t="inlineStr">
         <is>
-          <t>otros_pr_sm_exp_com_sex</t>
+          <t>otros_pr_sm_abu_sex</t>
         </is>
       </c>
       <c r="B3012">
@@ -68310,7 +68310,7 @@
     <row r="3013">
       <c r="A3013" t="inlineStr">
         <is>
-          <t>otros_pr_sm_exp_com_sex</t>
+          <t>otros_pr_sm_abu_sex</t>
         </is>
       </c>
       <c r="B3013">
@@ -68327,13 +68327,13 @@
         </is>
       </c>
       <c r="E3013">
-        <v>109066</v>
+        <v>107666</v>
       </c>
     </row>
     <row r="3014">
       <c r="A3014" t="inlineStr">
         <is>
-          <t>otros_pr_sm_exp_com_sex</t>
+          <t>otros_pr_sm_abu_sex</t>
         </is>
       </c>
       <c r="B3014">
@@ -68350,13 +68350,13 @@
         </is>
       </c>
       <c r="E3014">
-        <v>690</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="3015">
       <c r="A3015" t="inlineStr">
         <is>
-          <t>otros_pr_sm_otros</t>
+          <t>otros_pr_sm_exp_com_sex</t>
         </is>
       </c>
       <c r="B3015">
@@ -68369,7 +68369,7 @@
     <row r="3016">
       <c r="A3016" t="inlineStr">
         <is>
-          <t>otros_pr_sm_otros</t>
+          <t>otros_pr_sm_exp_com_sex</t>
         </is>
       </c>
       <c r="B3016">
@@ -68386,13 +68386,13 @@
         </is>
       </c>
       <c r="E3016">
-        <v>93864</v>
+        <v>109066</v>
       </c>
     </row>
     <row r="3017">
       <c r="A3017" t="inlineStr">
         <is>
-          <t>otros_pr_sm_otros</t>
+          <t>otros_pr_sm_exp_com_sex</t>
         </is>
       </c>
       <c r="B3017">
@@ -68409,13 +68409,13 @@
         </is>
       </c>
       <c r="E3017">
-        <v>15892</v>
+        <v>690</v>
       </c>
     </row>
     <row r="3018">
       <c r="A3018" t="inlineStr">
         <is>
-          <t>otros_pr_sm_vif</t>
+          <t>otros_pr_sm_otros</t>
         </is>
       </c>
       <c r="B3018">
@@ -68428,7 +68428,7 @@
     <row r="3019">
       <c r="A3019" t="inlineStr">
         <is>
-          <t>otros_pr_sm_vif</t>
+          <t>otros_pr_sm_otros</t>
         </is>
       </c>
       <c r="B3019">
@@ -68445,13 +68445,13 @@
         </is>
       </c>
       <c r="E3019">
-        <v>81888</v>
+        <v>93864</v>
       </c>
     </row>
     <row r="3020">
       <c r="A3020" t="inlineStr">
         <is>
-          <t>otros_pr_sm_vif</t>
+          <t>otros_pr_sm_otros</t>
         </is>
       </c>
       <c r="B3020">
@@ -68468,13 +68468,13 @@
         </is>
       </c>
       <c r="E3020">
-        <v>27868</v>
+        <v>15892</v>
       </c>
     </row>
     <row r="3021">
       <c r="A3021" t="inlineStr">
         <is>
-          <t>condicion_ocupacional_corr</t>
+          <t>otros_pr_sm_vif</t>
         </is>
       </c>
       <c r="B3021">
@@ -68487,7 +68487,7 @@
     <row r="3022">
       <c r="A3022" t="inlineStr">
         <is>
-          <t>condicion_ocupacional_corr</t>
+          <t>otros_pr_sm_vif</t>
         </is>
       </c>
       <c r="B3022">
@@ -68495,22 +68495,22 @@
       </c>
       <c r="C3022" t="inlineStr">
         <is>
-          <t>1.Employed</t>
+          <t>1.Absence</t>
         </is>
       </c>
       <c r="D3022" t="inlineStr">
         <is>
-          <t>Employed</t>
+          <t>Absence</t>
         </is>
       </c>
       <c r="E3022">
-        <v>50394</v>
+        <v>81888</v>
       </c>
     </row>
     <row r="3023">
       <c r="A3023" t="inlineStr">
         <is>
-          <t>condicion_ocupacional_corr</t>
+          <t>otros_pr_sm_vif</t>
         </is>
       </c>
       <c r="B3023">
@@ -68518,16 +68518,16 @@
       </c>
       <c r="C3023" t="inlineStr">
         <is>
-          <t>2.Inactive</t>
+          <t>2.Presence</t>
         </is>
       </c>
       <c r="D3023" t="inlineStr">
         <is>
-          <t>Inactive</t>
+          <t>Presence</t>
         </is>
       </c>
       <c r="E3023">
-        <v>11485</v>
+        <v>27868</v>
       </c>
     </row>
     <row r="3024">
@@ -68537,20 +68537,10 @@
         </is>
       </c>
       <c r="B3024">
-        <v>4</v>
-      </c>
-      <c r="C3024" t="inlineStr">
-        <is>
-          <t>3.Looking for a job for the first time</t>
-        </is>
-      </c>
-      <c r="D3024" t="inlineStr">
-        <is>
-          <t>Looking for a job for the first time</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E3024">
-        <v>233</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="3025">
@@ -68560,20 +68550,20 @@
         </is>
       </c>
       <c r="B3025">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3025" t="inlineStr">
         <is>
-          <t>4.No activity</t>
+          <t>1.Employed</t>
         </is>
       </c>
       <c r="D3025" t="inlineStr">
         <is>
-          <t>No activity</t>
+          <t>Employed</t>
         </is>
       </c>
       <c r="E3025">
-        <v>6811</v>
+        <v>50394</v>
       </c>
     </row>
     <row r="3026">
@@ -68583,20 +68573,20 @@
         </is>
       </c>
       <c r="B3026">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3026" t="inlineStr">
         <is>
-          <t>5.Not seeking for work</t>
+          <t>2.Inactive</t>
         </is>
       </c>
       <c r="D3026" t="inlineStr">
         <is>
-          <t>Not seeking for work</t>
+          <t>Inactive</t>
         </is>
       </c>
       <c r="E3026">
-        <v>1156</v>
+        <v>11485</v>
       </c>
     </row>
     <row r="3027">
@@ -68606,79 +68596,89 @@
         </is>
       </c>
       <c r="B3027">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3027" t="inlineStr">
         <is>
-          <t>6.Unemployed</t>
+          <t>3.Looking for a job for the first time</t>
         </is>
       </c>
       <c r="D3027" t="inlineStr">
         <is>
-          <t>Unemployed</t>
+          <t>Looking for a job for the first time</t>
         </is>
       </c>
       <c r="E3027">
-        <v>39676</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3028">
       <c r="A3028" t="inlineStr">
         <is>
-          <t>cat_ocupacional_corr</t>
+          <t>condicion_ocupacional_corr</t>
         </is>
       </c>
       <c r="B3028">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="C3028" t="inlineStr">
+        <is>
+          <t>4.No activity</t>
+        </is>
+      </c>
+      <c r="D3028" t="inlineStr">
+        <is>
+          <t>No activity</t>
+        </is>
       </c>
       <c r="E3028">
-        <v>9999999</v>
+        <v>6811</v>
       </c>
     </row>
     <row r="3029">
       <c r="A3029" t="inlineStr">
         <is>
-          <t>cat_ocupacional_corr</t>
+          <t>condicion_ocupacional_corr</t>
         </is>
       </c>
       <c r="B3029">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3029" t="inlineStr">
         <is>
-          <t>1.Employer</t>
+          <t>5.Not seeking for work</t>
         </is>
       </c>
       <c r="D3029" t="inlineStr">
         <is>
-          <t>Employer</t>
+          <t>Not seeking for work</t>
         </is>
       </c>
       <c r="E3029">
-        <v>1556</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="3030">
       <c r="A3030" t="inlineStr">
         <is>
-          <t>cat_ocupacional_corr</t>
+          <t>condicion_ocupacional_corr</t>
         </is>
       </c>
       <c r="B3030">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3030" t="inlineStr">
         <is>
-          <t>2.Other</t>
+          <t>6.Unemployed</t>
         </is>
       </c>
       <c r="D3030" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Unemployed</t>
         </is>
       </c>
       <c r="E3030">
-        <v>999</v>
+        <v>39676</v>
       </c>
     </row>
     <row r="3031">
@@ -68688,20 +68688,10 @@
         </is>
       </c>
       <c r="B3031">
-        <v>4</v>
-      </c>
-      <c r="C3031" t="inlineStr">
-        <is>
-          <t>3.Salaried</t>
-        </is>
-      </c>
-      <c r="D3031" t="inlineStr">
-        <is>
-          <t>Salaried</t>
-        </is>
+        <v>1</v>
       </c>
       <c r="E3031">
-        <v>30140</v>
+        <v>9999999</v>
       </c>
     </row>
     <row r="3032">
@@ -68711,20 +68701,20 @@
         </is>
       </c>
       <c r="B3032">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3032" t="inlineStr">
         <is>
-          <t>4.Self-employed</t>
+          <t>1.Employer</t>
         </is>
       </c>
       <c r="D3032" t="inlineStr">
         <is>
-          <t>Self-employed</t>
+          <t>Employer</t>
         </is>
       </c>
       <c r="E3032">
-        <v>13466</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="3033">
@@ -68734,20 +68724,20 @@
         </is>
       </c>
       <c r="B3033">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3033" t="inlineStr">
         <is>
-          <t>5.Unpaid family labour</t>
+          <t>2.Other</t>
         </is>
       </c>
       <c r="D3033" t="inlineStr">
         <is>
-          <t>Unpaid family labour</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="E3033">
-        <v>231</v>
+        <v>999</v>
       </c>
     </row>
     <row r="3034">
@@ -68757,19 +68747,88 @@
         </is>
       </c>
       <c r="B3034">
+        <v>4</v>
+      </c>
+      <c r="C3034" t="inlineStr">
+        <is>
+          <t>3.Salaried</t>
+        </is>
+      </c>
+      <c r="D3034" t="inlineStr">
+        <is>
+          <t>Salaried</t>
+        </is>
+      </c>
+      <c r="E3034">
+        <v>30140</v>
+      </c>
+    </row>
+    <row r="3035">
+      <c r="A3035" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3035">
+        <v>5</v>
+      </c>
+      <c r="C3035" t="inlineStr">
+        <is>
+          <t>4.Self-employed</t>
+        </is>
+      </c>
+      <c r="D3035" t="inlineStr">
+        <is>
+          <t>Self-employed</t>
+        </is>
+      </c>
+      <c r="E3035">
+        <v>13466</v>
+      </c>
+    </row>
+    <row r="3036">
+      <c r="A3036" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3036">
+        <v>6</v>
+      </c>
+      <c r="C3036" t="inlineStr">
+        <is>
+          <t>5.Unpaid family labour</t>
+        </is>
+      </c>
+      <c r="D3036" t="inlineStr">
+        <is>
+          <t>Unpaid family labour</t>
+        </is>
+      </c>
+      <c r="E3036">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3037">
+      <c r="A3037" t="inlineStr">
+        <is>
+          <t>cat_ocupacional_corr</t>
+        </is>
+      </c>
+      <c r="B3037">
         <v>7</v>
       </c>
-      <c r="C3034" t="inlineStr">
+      <c r="C3037" t="inlineStr">
         <is>
           <t>6.Volunteer worker</t>
         </is>
       </c>
-      <c r="D3034" t="inlineStr">
+      <c r="D3037" t="inlineStr">
         <is>
           <t>Volunteer worker</t>
         </is>
       </c>
-      <c r="E3034">
+      <c r="E3037">
         <v>196</v>
       </c>
     </row>

</xml_diff>